<commit_message>
+/- instruktora do pośredniej kolekcji
</commit_message>
<xml_diff>
--- a/Doc/Wykonane zadania.xlsx
+++ b/Doc/Wykonane zadania.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Spotkanie KEEPER.20140918</t>
   </si>
@@ -31,6 +31,12 @@
   </si>
   <si>
     <t>implementacja widoku aktualnego cennika pakietów medycznych (w kontekście daty procesowania widoku)</t>
+  </si>
+  <si>
+    <t>funkcja vba konwertująca polskie znaki na łacińskie</t>
+  </si>
+  <si>
+    <t>implementacja linii poleceń w LanguageCourseView</t>
   </si>
 </sst>
 </file>
@@ -67,8 +73,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -370,40 +377,86 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:O16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="110.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B2" s="1">
+        <v>41901</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B3" s="1">
+        <v>41901</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B4" s="1">
+        <v>41901</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>41901</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>41904</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>41904</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B8" s="1">
+        <v>41905</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O15" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O16">
+        <f>TRUNC(O15)</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>